<commit_message>
add qty to promotionCondition
</commit_message>
<xml_diff>
--- a/LaundryAnalysis.xlsx
+++ b/LaundryAnalysis.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\Waan\databaseSumana\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\Waan\LaundryService\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Promotion" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>สุดคุ้ม 20 ตัว</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>qty_item</t>
+  </si>
+  <si>
+    <t>CUS_ID</t>
   </si>
 </sst>
 </file>
@@ -292,10 +295,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T14" sqref="T14:T15"/>
     </sheetView>
   </sheetViews>
@@ -599,11 +602,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -744,7 +747,7 @@
       <c r="N17">
         <v>15</v>
       </c>
-      <c r="P17" s="8" t="s">
+      <c r="P17" s="7" t="s">
         <v>53</v>
       </c>
       <c r="Q17">
@@ -764,7 +767,7 @@
       <c r="N18">
         <v>20</v>
       </c>
-      <c r="P18" s="8" t="s">
+      <c r="P18" s="7" t="s">
         <v>55</v>
       </c>
       <c r="Q18">
@@ -772,19 +775,19 @@
       </c>
     </row>
     <row r="19" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="P19" s="8"/>
+      <c r="P19" s="7"/>
     </row>
     <row r="20" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="P20" s="8"/>
+      <c r="P20" s="7"/>
     </row>
     <row r="21" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="P21" s="8"/>
+      <c r="P21" s="7"/>
     </row>
     <row r="22" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="P22" s="8"/>
+      <c r="P22" s="7"/>
     </row>
     <row r="23" spans="11:17" x14ac:dyDescent="0.25">
-      <c r="P23" s="8"/>
+      <c r="P23" s="7"/>
     </row>
     <row r="27" spans="11:17" x14ac:dyDescent="0.25">
       <c r="L27" t="s">
@@ -1077,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,6 +1100,9 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>63</v>
+      </c>
       <c r="B2" t="s">
         <v>39</v>
       </c>
@@ -1117,8 +1123,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>19</v>
+      <c r="A3">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1142,8 +1148,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
+      <c r="A4">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>

</xml_diff>

<commit_message>
fixed parkage id no calculate monry
</commit_message>
<xml_diff>
--- a/LaundryAnalysis.xlsx
+++ b/LaundryAnalysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Promotion" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="GLฌศ์" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="65">
   <si>
     <t>สุดคุ้ม 20 ตัว</t>
   </si>
@@ -145,9 +146,6 @@
     <t>ODERSUB_ID</t>
   </si>
   <si>
-    <t>REGISTER + CUS_ID+ORDER_ID</t>
-  </si>
-  <si>
     <t>ORDER_ID</t>
   </si>
   <si>
@@ -221,6 +219,12 @@
   </si>
   <si>
     <t>CUS_ID</t>
+  </si>
+  <si>
+    <t>REGISTER + CUS_ID+RANDOM(6)</t>
+  </si>
+  <si>
+    <t>20170420-1-111</t>
   </si>
 </sst>
 </file>
@@ -700,7 +704,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -716,22 +720,22 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="11:17" x14ac:dyDescent="0.25">
@@ -748,7 +752,7 @@
         <v>15</v>
       </c>
       <c r="P17" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q17">
         <v>5</v>
@@ -759,7 +763,7 @@
         <v>2</v>
       </c>
       <c r="L18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -768,7 +772,7 @@
         <v>20</v>
       </c>
       <c r="P18" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q18">
         <v>-15</v>
@@ -791,12 +795,12 @@
     </row>
     <row r="27" spans="11:17" x14ac:dyDescent="0.25">
       <c r="L27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="11:17" x14ac:dyDescent="0.25">
       <c r="L28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M28">
         <v>1</v>
@@ -807,10 +811,10 @@
     </row>
     <row r="29" spans="11:17" x14ac:dyDescent="0.25">
       <c r="L29" t="s">
+        <v>56</v>
+      </c>
+      <c r="M29" t="s">
         <v>57</v>
-      </c>
-      <c r="M29" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -980,16 +984,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1034,7 +1038,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4">
         <v>20</v>
@@ -1054,7 +1058,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H5">
         <v>20</v>
@@ -1065,7 +1069,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H6">
         <v>80</v>
@@ -1078,16 +1082,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I5" sqref="I5:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1096,15 +1100,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -1130,17 +1134,17 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1">
         <v>43332</v>
       </c>
       <c r="E3" s="1">
-        <f>D3+3</f>
+        <f t="shared" ref="E3:E8" si="0">D3+3</f>
         <v>43335</v>
       </c>
       <c r="F3" s="1">
-        <f>D3+366</f>
+        <f t="shared" ref="F3:F8" si="1">D3+366</f>
         <v>43698</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -1155,20 +1159,120 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="D4" s="1">
         <v>43332</v>
       </c>
       <c r="E4" s="1">
-        <f>D4+3</f>
+        <f t="shared" si="0"/>
         <v>43335</v>
       </c>
       <c r="F4" s="1">
-        <f>D4+366</f>
+        <f t="shared" si="1"/>
         <v>43698</v>
       </c>
       <c r="G4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1">
+        <v>43332</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>43335</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
+        <v>43698</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1">
+        <v>43332</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>43335</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
+        <v>43698</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="1">
+        <v>43332</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>43335</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
+        <v>43698</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1">
+        <v>43332</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>43335</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>43698</v>
+      </c>
+      <c r="G8" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1206,7 +1310,7 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1296,18 +1400,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>10</v>
@@ -1331,7 +1435,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -1345,7 +1449,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6">
         <v>10</v>

</xml_diff>